<commit_message>
Updated Tidy Table and Finalized Code for Qiang_2020
</commit_message>
<xml_diff>
--- a/wishlist/Qiang_2020_IEEE/Qiang_2020_TT.xlsx
+++ b/wishlist/Qiang_2020_IEEE/Qiang_2020_TT.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/harrisondavis/Documents/GitHub/nmcuration/wishlist/Qiang_2020_IEEE/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41AD5F8-6ADE-A34C-A55F-610AC3FA2564}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27F96545-FAB8-7E44-965D-5D4BE1630808}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8900" yWindow="460" windowWidth="19640" windowHeight="17520" xr2:uid="{AB200291-E7E2-5D4B-81EA-6FBD7D80A147}"/>
   </bookViews>
@@ -35,12 +35,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="26">
   <si>
-    <t>Sample:</t>
-  </si>
-  <si>
-    <t>Control:</t>
-  </si>
-  <si>
     <t>S1</t>
   </si>
   <si>
@@ -71,12 +65,6 @@
     <t>S10</t>
   </si>
   <si>
-    <t>wt%</t>
-  </si>
-  <si>
-    <t>Datafiles</t>
-  </si>
-  <si>
     <t>AC_Weibull_Pure.xlsx</t>
   </si>
   <si>
@@ -111,6 +99,18 @@
   </si>
   <si>
     <t>Shape Parameter</t>
+  </si>
+  <si>
+    <t>Datafile</t>
+  </si>
+  <si>
+    <t>wt</t>
+  </si>
+  <si>
+    <t>Sample</t>
+  </si>
+  <si>
+    <t>Control</t>
   </si>
 </sst>
 </file>
@@ -488,7 +488,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -500,34 +500,34 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>0</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1</v>
+        <v>25</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1"/>
       <c r="D2" s="1" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="E2" s="1">
         <v>222.7</v>
@@ -538,16 +538,16 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C3" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="E3" s="1">
         <v>185.4</v>
@@ -558,16 +558,16 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C4" s="1">
         <v>0.01</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="E4" s="1">
         <v>184</v>
@@ -578,16 +578,16 @@
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C5" s="1">
         <v>0.03</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="E5" s="1">
         <v>183.9</v>
@@ -598,16 +598,16 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C6" s="1">
         <v>0.05</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="E6" s="1">
         <v>171.2</v>
@@ -618,14 +618,14 @@
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="E7" s="1">
         <v>502.1</v>
@@ -636,16 +636,16 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C8" s="1">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E8" s="1">
         <v>424.3</v>
@@ -656,16 +656,16 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C9" s="1">
         <v>0.01</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="E9" s="1">
         <v>441.4</v>
@@ -676,16 +676,16 @@
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C10" s="1">
         <v>0.03</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="E10" s="1">
         <v>373.3</v>
@@ -696,16 +696,16 @@
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C11" s="1">
         <v>0.05</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="E11" s="1">
         <v>332.2</v>

</xml_diff>